<commit_message>
final adjustments for pub
final adjustments for publication.
</commit_message>
<xml_diff>
--- a/data_out2020/List of Fragile Contexts (2020).xlsx
+++ b/data_out2020/List of Fragile Contexts (2020).xlsx
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.93428814719645</v>
+        <v>-4.93428814715969</v>
       </c>
     </row>
     <row r="3">
@@ -742,7 +742,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.71019887493815</v>
+        <v>-4.71019887494382</v>
       </c>
     </row>
     <row r="4">
@@ -756,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.51460469575541</v>
+        <v>-4.51460469579629</v>
       </c>
     </row>
     <row r="5">
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>-4.18989935930305</v>
+        <v>-4.18989935933375</v>
       </c>
     </row>
     <row r="6">
@@ -784,7 +784,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.89839320172937</v>
+        <v>-3.89839320168245</v>
       </c>
     </row>
     <row r="7">
@@ -798,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>-3.6111931008518</v>
+        <v>-3.611193100858</v>
       </c>
     </row>
     <row r="8">
@@ -812,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.50295530820229</v>
+        <v>-3.50295530817517</v>
       </c>
     </row>
     <row r="9">
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.49145131386435</v>
+        <v>-3.49145131390669</v>
       </c>
     </row>
     <row r="10">
@@ -840,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.374947291573</v>
+        <v>-3.37494729160697</v>
       </c>
     </row>
     <row r="11">
@@ -854,7 +854,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>-3.23977865660237</v>
+        <v>-3.23977865664204</v>
       </c>
     </row>
     <row r="12">
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.92817740560514</v>
+        <v>-2.92817740560075</v>
       </c>
     </row>
     <row r="13">
@@ -882,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.73189707579864</v>
+        <v>-2.73189707576306</v>
       </c>
     </row>
     <row r="14">
@@ -896,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.66020821057471</v>
+        <v>-2.66020821060716</v>
       </c>
     </row>
     <row r="15">
@@ -910,7 +910,7 @@
         <v>33</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.47366141848774</v>
+        <v>-2.47366141843785</v>
       </c>
     </row>
     <row r="16">
@@ -924,7 +924,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="n">
-        <v>-2.40213554420318</v>
+        <v>-2.40213554417025</v>
       </c>
     </row>
     <row r="17">
@@ -938,7 +938,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="n">
-        <v>-2.39741396468621</v>
+        <v>-2.39741396464398</v>
       </c>
     </row>
     <row r="18">
@@ -952,7 +952,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="n">
-        <v>-2.39725564619083</v>
+        <v>-2.39725564619074</v>
       </c>
     </row>
     <row r="19">
@@ -966,7 +966,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="n">
-        <v>-2.23478583147065</v>
+        <v>-2.23478583147039</v>
       </c>
     </row>
     <row r="20">
@@ -980,7 +980,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="n">
-        <v>-2.20884454729889</v>
+        <v>-2.20884454734835</v>
       </c>
     </row>
     <row r="21">
@@ -994,7 +994,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="n">
-        <v>-2.20798277996414</v>
+        <v>-2.20798277994734</v>
       </c>
     </row>
     <row r="22">
@@ -1008,7 +1008,7 @@
         <v>33</v>
       </c>
       <c r="D22" t="n">
-        <v>-2.13549141653403</v>
+        <v>-2.13549141653435</v>
       </c>
     </row>
     <row r="23">
@@ -1022,7 +1022,7 @@
         <v>33</v>
       </c>
       <c r="D23" t="n">
-        <v>-2.11675823211986</v>
+        <v>-2.11675823207754</v>
       </c>
     </row>
     <row r="24">
@@ -1036,7 +1036,7 @@
         <v>33</v>
       </c>
       <c r="D24" t="n">
-        <v>-2.11115062051144</v>
+        <v>-2.11115062051429</v>
       </c>
     </row>
     <row r="25">
@@ -1050,7 +1050,7 @@
         <v>33</v>
       </c>
       <c r="D25" t="n">
-        <v>-2.03610833541803</v>
+        <v>-2.03610833537792</v>
       </c>
     </row>
     <row r="26">
@@ -1064,7 +1064,7 @@
         <v>33</v>
       </c>
       <c r="D26" t="n">
-        <v>-1.9319603943058</v>
+        <v>-1.93196039433653</v>
       </c>
     </row>
     <row r="27">
@@ -1078,7 +1078,7 @@
         <v>33</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.92924945993456</v>
+        <v>-1.92924945998237</v>
       </c>
     </row>
     <row r="28">
@@ -1092,7 +1092,7 @@
         <v>33</v>
       </c>
       <c r="D28" t="n">
-        <v>-1.9111043401677</v>
+        <v>-1.91110434015121</v>
       </c>
     </row>
     <row r="29">
@@ -1106,7 +1106,7 @@
         <v>33</v>
       </c>
       <c r="D29" t="n">
-        <v>-1.9063814817741</v>
+        <v>-1.906381481786</v>
       </c>
     </row>
     <row r="30">
@@ -1120,7 +1120,7 @@
         <v>33</v>
       </c>
       <c r="D30" t="n">
-        <v>-1.89874320059088</v>
+        <v>-1.89874320062355</v>
       </c>
     </row>
     <row r="31">
@@ -1134,7 +1134,7 @@
         <v>33</v>
       </c>
       <c r="D31" t="n">
-        <v>-1.89551107248947</v>
+        <v>-1.89551107247236</v>
       </c>
     </row>
     <row r="32">
@@ -1148,7 +1148,7 @@
         <v>33</v>
       </c>
       <c r="D32" t="n">
-        <v>-1.8850070075654</v>
+        <v>-1.88500700753677</v>
       </c>
     </row>
     <row r="33">
@@ -1162,7 +1162,7 @@
         <v>33</v>
       </c>
       <c r="D33" t="n">
-        <v>-1.87225883786938</v>
+        <v>-1.87225883790481</v>
       </c>
     </row>
     <row r="34">
@@ -1176,7 +1176,7 @@
         <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>-1.83233988322998</v>
+        <v>-1.8323398832478</v>
       </c>
     </row>
     <row r="35">
@@ -1190,7 +1190,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="n">
-        <v>-1.83013095687076</v>
+        <v>-1.83013095690854</v>
       </c>
     </row>
     <row r="36">
@@ -1204,7 +1204,7 @@
         <v>33</v>
       </c>
       <c r="D36" t="n">
-        <v>-1.82752120952668</v>
+        <v>-1.82752120952425</v>
       </c>
     </row>
     <row r="37">
@@ -1218,7 +1218,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="n">
-        <v>-1.80740467767441</v>
+        <v>-1.80740467765807</v>
       </c>
     </row>
     <row r="38">
@@ -1232,7 +1232,7 @@
         <v>33</v>
       </c>
       <c r="D38" t="n">
-        <v>-1.80125247164303</v>
+        <v>-1.80125247164438</v>
       </c>
     </row>
     <row r="39">
@@ -1246,7 +1246,7 @@
         <v>33</v>
       </c>
       <c r="D39" t="n">
-        <v>-1.79837077022521</v>
+        <v>-1.79837077016943</v>
       </c>
     </row>
     <row r="40">
@@ -1260,7 +1260,7 @@
         <v>33</v>
       </c>
       <c r="D40" t="n">
-        <v>-1.78913231166291</v>
+        <v>-1.78913231168957</v>
       </c>
     </row>
     <row r="41">
@@ -1274,7 +1274,7 @@
         <v>33</v>
       </c>
       <c r="D41" t="n">
-        <v>-1.75801147548215</v>
+        <v>-1.75801147547518</v>
       </c>
     </row>
     <row r="42">
@@ -1288,7 +1288,7 @@
         <v>33</v>
       </c>
       <c r="D42" t="n">
-        <v>-1.74510541950755</v>
+        <v>-1.74510541952819</v>
       </c>
     </row>
     <row r="43">
@@ -1302,7 +1302,7 @@
         <v>33</v>
       </c>
       <c r="D43" t="n">
-        <v>-1.74338985314878</v>
+        <v>-1.74338985317171</v>
       </c>
     </row>
     <row r="44">
@@ -1316,7 +1316,7 @@
         <v>33</v>
       </c>
       <c r="D44" t="n">
-        <v>-1.70113343984272</v>
+        <v>-1.70113343984342</v>
       </c>
     </row>
     <row r="45">
@@ -1330,7 +1330,7 @@
         <v>33</v>
       </c>
       <c r="D45" t="n">
-        <v>-1.66042950526625</v>
+        <v>-1.66042950527787</v>
       </c>
     </row>
     <row r="46">
@@ -1344,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="D46" t="n">
-        <v>-1.62167423878497</v>
+        <v>-1.62167423878348</v>
       </c>
     </row>
     <row r="47">
@@ -1358,7 +1358,7 @@
         <v>33</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.5942642461041</v>
+        <v>-1.59426424614002</v>
       </c>
     </row>
     <row r="48">
@@ -1372,7 +1372,7 @@
         <v>33</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.55235318041862</v>
+        <v>-1.55235318045711</v>
       </c>
     </row>
     <row r="49">
@@ -1386,7 +1386,7 @@
         <v>33</v>
       </c>
       <c r="D49" t="n">
-        <v>-1.52604152975796</v>
+        <v>-1.52604152974272</v>
       </c>
     </row>
     <row r="50">
@@ -1400,7 +1400,7 @@
         <v>33</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.47408876655164</v>
+        <v>-1.47408876659324</v>
       </c>
     </row>
     <row r="51">
@@ -1414,7 +1414,7 @@
         <v>33</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.44334427359872</v>
+        <v>-1.44334427356975</v>
       </c>
     </row>
     <row r="52">
@@ -1428,7 +1428,7 @@
         <v>33</v>
       </c>
       <c r="D52" t="n">
-        <v>-1.43329910126417</v>
+        <v>-1.43329910130259</v>
       </c>
     </row>
     <row r="53">
@@ -1442,7 +1442,7 @@
         <v>33</v>
       </c>
       <c r="D53" t="n">
-        <v>-1.37729086752988</v>
+        <v>-1.37729086752435</v>
       </c>
     </row>
     <row r="54">
@@ -1456,7 +1456,7 @@
         <v>33</v>
       </c>
       <c r="D54" t="n">
-        <v>-1.36985696216637</v>
+        <v>-1.36985696215215</v>
       </c>
     </row>
     <row r="55">
@@ -1470,7 +1470,7 @@
         <v>33</v>
       </c>
       <c r="D55" t="n">
-        <v>-1.3686440793618</v>
+        <v>-1.36864407931386</v>
       </c>
     </row>
     <row r="56">
@@ -1484,7 +1484,7 @@
         <v>33</v>
       </c>
       <c r="D56" t="n">
-        <v>-1.28230080167068</v>
+        <v>-1.28230080169039</v>
       </c>
     </row>
     <row r="57">
@@ -1498,7 +1498,7 @@
         <v>33</v>
       </c>
       <c r="D57" t="n">
-        <v>-1.23435126873152</v>
+        <v>-1.23435126875711</v>
       </c>
     </row>
     <row r="58">
@@ -1512,7 +1512,7 @@
         <v>33</v>
       </c>
       <c r="D58" t="n">
-        <v>-1.21670478683775</v>
+        <v>-1.2167047867817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>